<commit_message>
Enhanced Import from Excel
</commit_message>
<xml_diff>
--- a/staticfiles/downloads/sample.xlsx
+++ b/staticfiles/downloads/sample.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27809"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28028"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joece\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joece\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FAC53AC-FACC-4E14-8030-E968B8BD87DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A829F6-8B62-4987-8F09-AD00438AC935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ABEEE02B-1BF2-4C8C-8491-A8EBC5AB8805}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{ABEEE02B-1BF2-4C8C-8491-A8EBC5AB8805}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Listings" sheetId="1" r:id="rId1"/>
+    <sheet name="Instructions" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Instructions!$B$2:$E$32</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,76 +40,177 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="44">
+  <si>
+    <t>Starting Bid</t>
+  </si>
+  <si>
+    <t>Reserve Bid</t>
+  </si>
+  <si>
+    <t>Auction Duration</t>
+  </si>
+  <si>
+    <t>Reference Number</t>
+  </si>
+  <si>
+    <t>Lot Number</t>
+  </si>
+  <si>
+    <t>Expiration Date</t>
+  </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Starting Bid</t>
-  </si>
-  <si>
-    <t>Reserve Bid</t>
-  </si>
-  <si>
-    <t>Auction Duration</t>
-  </si>
-  <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>Reference Number</t>
-  </si>
-  <si>
-    <t>Lot Number</t>
-  </si>
-  <si>
-    <t>Expiration Date</t>
-  </si>
-  <si>
-    <t>Package Type</t>
-  </si>
-  <si>
-    <t>Package Quantity</t>
-  </si>
-  <si>
-    <t>Device Sterile</t>
-  </si>
-  <si>
-    <t>Full Package</t>
-  </si>
-  <si>
-    <t>Test auction 4</t>
-  </si>
-  <si>
-    <t>Test desc</t>
-  </si>
-  <si>
-    <t>Cate</t>
-  </si>
-  <si>
-    <t>Bob</t>
-  </si>
-  <si>
-    <t>123abc</t>
-  </si>
-  <si>
-    <t>123ccc</t>
-  </si>
-  <si>
-    <t>Box</t>
-  </si>
-  <si>
-    <t>Product Name</t>
+    <t>SKU</t>
+  </si>
+  <si>
+    <t>Production Date</t>
+  </si>
+  <si>
+    <t>Auction Type</t>
+  </si>
+  <si>
+    <t>Sale Price</t>
+  </si>
+  <si>
+    <t>Quantity Available</t>
+  </si>
+  <si>
+    <t>Field Name</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Allowed Values</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>A unique identifier for the product.</t>
+  </si>
+  <si>
+    <t>Any text or number.</t>
+  </si>
+  <si>
+    <t>A reference number associated with the product.</t>
+  </si>
+  <si>
+    <t>A lot number associated with the product.</t>
+  </si>
+  <si>
+    <t>The date when the product was produced.</t>
+  </si>
+  <si>
+    <t>Date format (YYYY-MM-DD).</t>
+  </si>
+  <si>
+    <t>The date when the product will expire.</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>The total quantity available for the listing.</t>
+  </si>
+  <si>
+    <t>Any positive integer.</t>
+  </si>
+  <si>
+    <t>The type of auction or sale.</t>
+  </si>
+  <si>
+    <t>"Auction" or "Sale".</t>
+  </si>
+  <si>
+    <t>The starting bid amount for the auction.</t>
+  </si>
+  <si>
+    <t>Any decimal value, e.g., 10.00.</t>
+  </si>
+  <si>
+    <t>The minimum bid amount required to complete the sale.</t>
+  </si>
+  <si>
+    <t>Any decimal value, e.g., 100.00.</t>
+  </si>
+  <si>
+    <t>The fixed price at which the product can be sold immediately.</t>
+  </si>
+  <si>
+    <t>Any decimal value, e.g., 150.00.</t>
+  </si>
+  <si>
+    <t>The duration of the auction in days.</t>
+  </si>
+  <si>
+    <t>1, 3, 5, 7, 10</t>
+  </si>
+  <si>
+    <t>Welcome to the Bulk Auction Import Tool! This template allows you to quickly and easily create multiple auction or sale listings by filling out the information in the table below. Each row represents a separate listing, so you can manage everything in one place. Follow the instructions in the 'Instructions' tab to ensure all your data is entered correctly, and let us handle the rest. Happy listing!</t>
+  </si>
+  <si>
+    <t>Auction Type Instructions</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>When setting up your listings, it's important to understand the difference between the 'Auction' and 'Sale' types:</t>
+  </si>
+  <si>
+    <t>Make sure to select the appropriate type for your listing to ensure all necessary fields are correctly filled out</t>
+  </si>
+  <si>
+    <r>
+      <t>Auction Type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: If you select 'Auction' as the listing type, you are required to provide values for both the 'Starting Bid' and 'Reserve Bid' fields. The 'Starting Bid' is the minimum amount the auction will begin at, and the 'Reserve Bid' is the minimum amount required for the sale to be completed.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sale Type:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> If you select 'Sale' as the listing type, the 'Starting Bid' and 'Reserve Bid' fields are not required. Instead, you'll need to provide a 'Sale Price,' which is the fixed price at which the product can be sold immediately.</t>
+    </r>
+  </si>
+  <si>
+    <t>Field Types and Allowed Values</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,16 +218,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -130,18 +272,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="3"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -474,118 +651,386 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE8C051-F048-40EC-A279-14AD87412FA2}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="17.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-      <c r="F2">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="2">
-        <v>44920</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2">
-        <v>12</v>
-      </c>
-      <c r="M2" t="b">
-        <v>1</v>
-      </c>
-      <c r="N2" t="b">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9463DFB9-E974-4A7A-8183-7D7DA7376D13}">
+  <dimension ref="B2:E32"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.85546875" customWidth="1"/>
+    <col min="5" max="5" width="35.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="2:5" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="B7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+    </row>
+    <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+    </row>
+    <row r="16" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+    </row>
+    <row r="19" spans="2:5" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="B19" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="B13:E14"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B3:E5"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B10:E11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="65" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>